<commit_message>
A strong password generation feature was added and the code became more efficient.The numeric password appears in the excel table, however the strong one doesn’t yet(I will make it appear in the future).
</commit_message>
<xml_diff>
--- a/all_passwords.xlsx
+++ b/all_passwords.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A102"/>
+  <dimension ref="A1:A52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,714 +424,364 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Passwords</t>
+          <t>Passwords-4 digit_numbers</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0336</t>
+          <t>0071</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3738</t>
+          <t>0142</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8637</t>
+          <t>3491</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>1496</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3752</t>
+          <t>2577</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>9517</t>
+          <t>5554</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1457</t>
+          <t>1972</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>9368</t>
+          <t>3457</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3827</t>
+          <t>3499</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3799</t>
+          <t>5363</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0500</t>
+          <t>9071</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>7862</t>
+          <t>6155</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0921</t>
+          <t>6405</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>6328</t>
+          <t>7320</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4167</t>
+          <t>9351</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4712</t>
+          <t>5497</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>4611</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4137</t>
+          <t>8928</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5792</t>
+          <t>8072</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>7026</t>
+          <t>4384</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5344</t>
+          <t>4339</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5203</t>
+          <t>6381</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1548</t>
+          <t>4815</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>8011</t>
+          <t>4873</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>7599</t>
+          <t>8569</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>7825</t>
+          <t>9442</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2658</t>
+          <t>9104</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>7909</t>
+          <t>4227</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6463</t>
+          <t>5121</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5225</t>
+          <t>1910</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6980</t>
+          <t>4590</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>8562</t>
+          <t>0888</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>8776</t>
+          <t>8419</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6934</t>
+          <t>9853</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>8832</t>
+          <t>8717</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6953</t>
+          <t>3216</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2579</t>
+          <t>7527</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2855</t>
+          <t>6172</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6042</t>
+          <t>0104</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2550</t>
+          <t>9038</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2298</t>
+          <t>9635</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2080</t>
+          <t>7391</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2974</t>
+          <t>9156</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0364</t>
+          <t>4761</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2834</t>
+          <t>4221</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>7618</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>4442</t>
+          <t>6982</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1492</t>
+          <t>0144</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5989</t>
+          <t>8445</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6603</t>
+          <t>7224</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6618</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>0232</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>1988</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>5574</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>0529</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>9324</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>8962</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>3567</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>6814</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>9197</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>3609</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>1178</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>9559</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>1206</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>2596</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>1163</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>4108</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>9809</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>4347</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>0606</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>1735</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>7457</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>6279</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>6797</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>7123</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>5143</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>7968</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>4432</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>4811</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>0521</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>6006</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>7176</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>6451</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>7411</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>0811</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>6626</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>2219</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>9257</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>8805</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>1920</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>8339</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>7133</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>8674</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>4668</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>0313</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>3200</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>3577</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>1863</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>6840</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>3726</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>5417</t>
+          <t>4877</t>
         </is>
       </c>
     </row>

</xml_diff>